<commit_message>
fixed twitter feed centering, changed some data + added facebook
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>cand_name</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>twitter_widget</t>
+  </si>
+  <si>
+    <t>fb</t>
   </si>
   <si>
     <t>Aspen Dunaway</t>
@@ -1957,7 +1960,9 @@
       <c r="N1" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="O1" s="6"/>
+      <c r="O1" t="s" s="5">
+        <v>14</v>
+      </c>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="7"/>
@@ -1972,44 +1977,44 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" t="s" s="15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s" s="16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s" s="17">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s" s="19">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O2" s="20"/>
       <c r="P2" s="21"/>
@@ -2026,44 +2031,44 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="s" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" t="s" s="25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s" s="17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s" s="19">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="21"/>
@@ -2080,44 +2085,44 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" t="s" s="26">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s" s="27">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s" s="17">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" t="s" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" t="s" s="19">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O4" s="20"/>
       <c r="P4" s="21"/>
@@ -2134,39 +2139,39 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="24">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" t="s" s="15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s" s="16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J5" s="28"/>
       <c r="K5" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="20"/>
@@ -2184,44 +2189,44 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" t="s" s="25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s" s="17">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K6" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M6" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N6" t="s" s="19">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O6" s="20"/>
       <c r="P6" s="21"/>
@@ -2238,44 +2243,44 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" t="s" s="26">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s" s="27">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s" s="17">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L7" t="s" s="18">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" t="s" s="19">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O7" s="20"/>
       <c r="P7" s="21"/>
@@ -2292,44 +2297,44 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" t="s" s="15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s" s="16">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" t="s" s="17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s" s="17">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K8" t="s" s="17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L8" t="s" s="40">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M8" t="s" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N8" t="s" s="19">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="21"/>

</xml_diff>

<commit_message>
cleaned js + some main templating issues
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>cand_name</t>
   </si>
@@ -61,7 +61,7 @@
     <t>Aspen Dunaway</t>
   </si>
   <si>
-    <t>Lorem</t>
+    <t>Attorney</t>
   </si>
   <si>
     <t>Ipsum Dolor</t>
@@ -70,18 +70,10 @@
     <t>https://twitter.com/dunawayfortexas</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="13"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>http://www.google.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Photo courtesy of the candidate</t>
+    <t>http://www.dunawayfortexas.com</t>
+  </si>
+  <si>
+    <t>Rachel Zein</t>
   </si>
   <si>
     <t>https://pbs.twimg.com/profile_images/600314410003865600/laIuu4bB.jpg</t>
@@ -93,18 +85,30 @@
     <t>Huey Rey Fischer</t>
   </si>
   <si>
+    <t>Former legislative aide</t>
+  </si>
+  <si>
     <t>https://twitter.com/HueyFischer</t>
   </si>
   <si>
+    <t>http://hueyfischer.com</t>
+  </si>
+  <si>
     <t>698624014843916288</t>
   </si>
   <si>
     <t>Gina Hinojosa</t>
   </si>
   <si>
+    <t>Austin ISD School Board member</t>
+  </si>
+  <si>
     <t>https://twitter.com/GinaForAustin</t>
   </si>
   <si>
+    <t>http://www.ginaforaustin.com</t>
+  </si>
+  <si>
     <t>698630662484418561</t>
   </si>
   <si>
@@ -114,19 +118,40 @@
     <t>Blake Rocap</t>
   </si>
   <si>
+    <t>Former NARAL Pro-Choice Texas counsel</t>
+  </si>
+  <si>
     <t>https://twitter.com/BlakeRocap</t>
   </si>
   <si>
+    <t>http://www.blakerocap.com</t>
+  </si>
+  <si>
+    <t>Blake Rocap campaign</t>
+  </si>
+  <si>
     <t>698630545312346112</t>
   </si>
   <si>
     <t>Matt Shrum</t>
   </si>
   <si>
+    <t>http://www.mattshrumfortexas.com</t>
+  </si>
+  <si>
     <t>Heather Way</t>
   </si>
   <si>
+    <t>University of Texas law professor</t>
+  </si>
+  <si>
     <t>https://twitter.com/hwayaustin</t>
+  </si>
+  <si>
+    <t>http://www.voteheatherway.com</t>
+  </si>
+  <si>
+    <t>Heather Way campaign</t>
   </si>
   <si>
     <t>698630136896172032</t>
@@ -161,20 +186,20 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="11"/>
       <color indexed="14"/>
       <name val="Arial"/>
     </font>
     <font>
       <u val="single"/>
-      <sz val="11"/>
-      <color indexed="13"/>
+      <sz val="10"/>
+      <color indexed="14"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -184,7 +209,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="14"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -649,10 +674,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -661,121 +686,121 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -808,8 +833,8 @@
       <rgbColor rgb="ffcccccc"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffff9900"/>
+      <rgbColor rgb="ff222222"/>
       <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ff222222"/>
       <rgbColor rgb="ff232323"/>
       <rgbColor rgb="ff1155cc"/>
     </indexedColors>
@@ -2029,7 +2054,7 @@
       </c>
       <c r="B3" s="21"/>
       <c r="C3" t="s" s="25">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s" s="17">
         <v>17</v>
@@ -2050,10 +2075,10 @@
         <v>17</v>
       </c>
       <c r="J3" t="s" s="17">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s" s="17">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s" s="18">
         <v>20</v>
@@ -2062,7 +2087,7 @@
         <v>21</v>
       </c>
       <c r="N3" t="s" s="19">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O3" s="20"/>
       <c r="P3" s="21"/>
@@ -2079,11 +2104,11 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="24">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" t="s" s="26">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s" s="27">
         <v>17</v>
@@ -2104,10 +2129,10 @@
         <v>17</v>
       </c>
       <c r="J4" t="s" s="17">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s" s="17">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s" s="18">
         <v>20</v>
@@ -2116,7 +2141,7 @@
         <v>21</v>
       </c>
       <c r="N4" t="s" s="19">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="O4" s="20"/>
       <c r="P4" s="21"/>
@@ -2133,7 +2158,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="24">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" t="s" s="15">
@@ -2158,12 +2183,8 @@
         <v>17</v>
       </c>
       <c r="J5" s="28"/>
-      <c r="K5" t="s" s="17">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s" s="18">
-        <v>20</v>
-      </c>
+      <c r="K5" s="17"/>
+      <c r="L5" s="18"/>
       <c r="M5" t="s" s="19">
         <v>21</v>
       </c>
@@ -2183,11 +2204,11 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" t="s" s="25">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s" s="17">
         <v>17</v>
@@ -2208,19 +2229,19 @@
         <v>17</v>
       </c>
       <c r="J6" t="s" s="17">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s" s="17">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="L6" t="s" s="18">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="M6" t="s" s="19">
         <v>21</v>
       </c>
       <c r="N6" t="s" s="19">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O6" s="20"/>
       <c r="P6" s="21"/>
@@ -2237,7 +2258,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" t="s" s="26">
@@ -2263,11 +2284,9 @@
       </c>
       <c r="J7" s="28"/>
       <c r="K7" t="s" s="17">
-        <v>19</v>
-      </c>
-      <c r="L7" t="s" s="18">
-        <v>20</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="L7" s="18"/>
       <c r="M7" t="s" s="19">
         <v>21</v>
       </c>
@@ -2287,11 +2306,11 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" t="s" s="15">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s" s="16">
         <v>17</v>
@@ -2312,19 +2331,19 @@
         <v>17</v>
       </c>
       <c r="J8" t="s" s="17">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K8" t="s" s="17">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="L8" t="s" s="40">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="M8" t="s" s="19">
         <v>21</v>
       </c>
       <c r="N8" t="s" s="19">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="O8" s="20"/>
       <c r="P8" s="21"/>
@@ -4020,15 +4039,6 @@
       <c r="Z68" s="63"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="K3" r:id="rId2" location="" tooltip="" display=""/>
-    <hyperlink ref="K4" r:id="rId3" location="" tooltip="" display=""/>
-    <hyperlink ref="K5" r:id="rId4" location="" tooltip="" display=""/>
-    <hyperlink ref="K6" r:id="rId5" location="" tooltip="" display=""/>
-    <hyperlink ref="K7" r:id="rId6" location="" tooltip="" display=""/>
-    <hyperlink ref="K8" r:id="rId7" location="" tooltip="" display=""/>
-  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
finalized build, some style changes
</commit_message>
<xml_diff>
--- a/backend/dataset.xlsx
+++ b/backend/dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>cand_name</t>
   </si>
@@ -70,6 +70,33 @@
     <t>The candidate has not provided the Daily Texan with this information.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>To find a full list of Aspen's endorsers, click &lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>http://www.dunawayfortexas.com/endorsements.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&gt;here&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
     <t>I came out of college in Texas with more than 50,000 in student loan debt.  I am fortunate to have them now paid off, but many of our young adults are not and will continue to struggle with making payments, and having looming debt over their heads. I am proposing a freeze on state university tuitions for a couple of years. I am also willing to look into re-regulating tuition.  I want to raise the minimum wage tax to at least $10.10 and make the steps needed to decriminalize marijuana.  I am also proposing a Tenant’s Bill of Rights. Texas has some protections in statute but they need to be clarified and disclosed to renters. Some provisions to the Bill of Rights include: security deposit not exceeding one month’s rent, a tenant right to privacy statute and adding to discrimination protection to include sexual orientation and marital status.  All these and more I have provided in my Formula for HD 49 and promised to file legislation on, fight for and support when elected.  I want what is best for the State but specifically I will be in that legislature representing and seeking what is best for HD 49, including UT and its students.  I will work with and alongside all constituents from students and young professionals to seniors and the disabled. I based this campaign on keeping this seat in the hands of the people and that is what I intend to do.</t>
   </si>
   <si>
@@ -97,6 +124,9 @@
     <t>698630836208345088</t>
   </si>
   <si>
+    <t>https://www.facebook.com/DunawayForTexas/?fref=ts</t>
+  </si>
+  <si>
     <t>Huey Rey Fischer</t>
   </si>
   <si>
@@ -106,6 +136,45 @@
     <t>Former legislative aide</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>University Democrats, Stonewall Democrats of Austin, The Victory Fund, Farm and Ranch Freedom Alliance, Austin Young Democrats. To find a full list of Huey's endorsers, click &lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>http://hueyfischer.com/supporters/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&gt;here&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>I’m different because these fights are personal for me. I am the recent UT grad who has significant student loan debt. I relied on Planned Parenthood for some health care screenings in college when I didn’t have health insurance. I can personally attest to the rising rent we are feeling in West and North Campus.&lt;br&gt;&lt;br&gt;I am the 23-year old, queer Latino taking on six lawyers for this seat. Students have been shut out of the Capitol for too long, and I am ready to push back with an agenda that is meaningful for the Forty Acres.&lt;br&gt;&lt;br&gt;The Legislature should fully fund the university to tackle the student debt crisis. We need to make student neighborhoods affordable again. We must begin a serious conversation about policies that will effectively end sexual assaults on campus. We have to keep guns out of our classrooms.&lt;br&gt;&lt;br&gt;Students will decide this election, and I am proud to be their choice.</t>
+  </si>
+  <si>
+    <t>Making Austin affordable</t>
+  </si>
+  <si>
+    <t>Tackling student debt</t>
+  </si>
+  <si>
+    <t>Fighting for social justice</t>
+  </si>
+  <si>
     <t>https://twitter.com/HueyFischer</t>
   </si>
   <si>
@@ -118,6 +187,9 @@
     <t>698624014843916288</t>
   </si>
   <si>
+    <t>https://www.facebook.com/HueyReyFischer/?fref=ts</t>
+  </si>
+  <si>
     <t>Gina Hinojosa</t>
   </si>
   <si>
@@ -127,6 +199,45 @@
     <t>Austin ISD School Board member</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>The Austin American-Statesman, Central Austin Democrats, Workers Defense Action Fund, Austin Chronicle, National Women's Political Caucus, West Austin Democrats. To find a full list of Gina's endorsers, click &lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>http://www.ginaforaustin.com/new-page/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&gt;here&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>We must not let Republicans roll back the clock on civil rights, women’s health, voting rights, the environment, and education – all issues that have a significant impact on the lives and future of students. I have a proven record of working successfully with coalitions to get things done, and I will collaborate with student organizations to fight for progressive issues at the State Capitol.&lt;br&gt;&lt;br&gt;I will work to make college opportunities affordable and more accessible for all students and ease the burden of student debt.&lt;br&gt;&lt;br&gt;The Texas Legislature is shortchanging young people and limiting their opportunities for an affordable college education and meaningful careers.  In the 1970’s, 85% of the education costs at the University of Texas were paid with state funds.  Today, the state share is less than 20%.  Students are caught in the squeeze, and the result is unprecedented student debt that has a profound impact on the social and economic mobility of young people today.&lt;br&gt;&lt;br&gt;I will SUPPORT:  Increased funding for the Texas Grants to increase college access for eligible students. OPPOSE:  Efforts to deny Dreamers in-state tuition and a shot at their future. SUPPORT:  Increased state share of costs for higher education to drive down tuition and ease student debt. SUPPORT:  Efforts to increase affordable student housing at UT.&lt;br&gt;&lt;br&gt;In addition, students are a key part of a progressive statewide coalition on issues such as: the environment - to address climate change; gun violence – to repeal campus carry; women’s reproductive rights - to fully restore funds to Planned Parenthood; and voting rights – to repeal voter ID laws.</t>
+  </si>
+  <si>
+    <t>We must end the epidemic of gun violence in Texas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We must stop shortchanging students </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We must restore full funding to Planned Parenthood </t>
+  </si>
+  <si>
     <t>https://twitter.com/GinaForAustin</t>
   </si>
   <si>
@@ -139,12 +250,21 @@
     <t>698630662484418561</t>
   </si>
   <si>
+    <t>https://www.facebook.com/GinaForAustin/?fref=ts</t>
+  </si>
+  <si>
     <t>Kenton Johnson</t>
   </si>
   <si>
     <t>johnson</t>
   </si>
   <si>
+    <t>default.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Kenton-D-Johnson-1660361334238015/?fref=ts</t>
+  </si>
+  <si>
     <t>Blake Rocap</t>
   </si>
   <si>
@@ -175,21 +295,39 @@
     <t>Blake Rocap campaign</t>
   </si>
   <si>
+    <t>rocap.jpg</t>
+  </si>
+  <si>
     <t>698630545312346112</t>
   </si>
   <si>
+    <t>https://www.facebook.com/VoteRocap/?fref=ts</t>
+  </si>
+  <si>
     <t>Matt Shrum</t>
   </si>
   <si>
     <t>shrum</t>
   </si>
   <si>
-    <t xml:space="preserve">Of the 7 candidates running, I am the most pragmatic which will make me the most effective advocate for district 49.  My experience at the Capitol tells me that in order to get things done over there, you have to be willing and able to work with the leadership.  That means holding on to your core values while reaching across the aisle and making compromises. </t>
+    <t xml:space="preserve">I do not have any of the traditional democratic club endorsements.  Nor have I actively sought them. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Of the seven candidates running, I am the most pragmatic which will make me the most effective advocate for district 49. My experience at the Capitol tells me that in order to get things done over there, you have to be willing and able to work with the leadership. That means holding on to your core values while reaching across the aisle and making compromises. </t>
   </si>
   <si>
     <t>http://www.mattshrumfortexas.com</t>
   </si>
   <si>
+    <t>Matt Shrum campaign</t>
+  </si>
+  <si>
+    <t>shrum.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/MattShrumforTexasHouse/?fref=ts</t>
+  </si>
+  <si>
     <t>Heather Way</t>
   </si>
   <si>
@@ -199,7 +337,34 @@
     <t>University of Texas law professor</t>
   </si>
   <si>
-    <t xml:space="preserve">As a UT Law professor, I have spent the past 10 years working closely with students and supporting their academic and personal growth (I was also a UT student for 7 years).  On a daily basis, I see UT students, staff, and faculty struggling to cope with dwindling recourses in an increasingly unaffordable city. As the Representative for District 49, I will be a champion at the Capitol for issues that are important to UT students, including increasing state investment in universities and making college affordable for all students, banning guns from our campus, expanding access to affordable rental housing, increasing student participation in the political process, and protecting women’s reproductive rights.&lt;br&gt;&lt;br&gt; I have dedicated my career to fighting for people and working to increase social and economic justice in our society.  I have a long successful record of standing up for our community here in Austin and at the Legislature—and getting results. I have worked as a legislative aide at the Capitol and have spent many years at the Capitol as a policy reformer.&lt;br&gt;&lt;br&gt;  I have the breadth of experience, knowledge, and dedication needed to achieve real reforms at the Capitol. </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>To find a full list of Heather's endorsers, click &lt;a href=</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="13"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>http://www.voteheatherway.com/supporters/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&gt;here&lt;/a&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>As a UT Law professor, I have spent the past 10 years working closely with students and supporting their academic and personal growth (I was also a UT student for seven years).  On a daily basis, I see UT students, staff, and faculty struggling to cope with dwindling recourses in an increasingly unaffordable city. As the Representative for District 49, I will be a champion at the Capitol for issues that are important to UT students, including increasing state investment in universities and making college affordable for all students, banning guns from our campus, expanding access to affordable rental housing, increasing student participation in the political process, and protecting women’s reproductive rights.&lt;br&gt;&lt;br&gt;I have dedicated my career to fighting for people and working to increase social and economic justice in our society.  I have a long successful record of standing up for our community here in Austin and at the Legislature—and getting results. I have worked as a legislative aide at the Capitol and have spent many years at the Capitol as a policy reformer.  I have the breadth of experience, knowledge, and dedication needed to achieve real reforms at the Capitol. &lt;br&gt;&lt;br&gt;I am also the only candidate stressing that we also need deep structural reforms to our political system—and leaders strong enough to stand up to the status quo. I will fight to get rid of corporate money in politics, increase transparency in government, and ban sweetheart deals for donors.</t>
   </si>
   <si>
     <t>Increasing economic opportunity and closing our society’s growing economic divides—through increasing investments in education, tax reform, adopting a living wage, affordable housing, and more</t>
@@ -224,6 +389,9 @@
   </si>
   <si>
     <t>698630136896172032</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/voteheatherway/?fref=ts</t>
   </si>
 </sst>
 </file>
@@ -255,20 +423,20 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <u val="single"/>
+      <sz val="10"/>
       <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="11"/>
       <color indexed="14"/>
       <name val="Arial"/>
     </font>
     <font>
       <u val="single"/>
-      <sz val="10"/>
-      <color indexed="14"/>
+      <sz val="11"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -278,7 +446,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="13"/>
+      <color indexed="14"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -302,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -460,6 +628,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -488,11 +665,20 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -688,7 +874,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -740,142 +926,154 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -899,8 +1097,8 @@
       <rgbColor rgb="ffcccccc"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffff9900"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff222222"/>
-      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff232323"/>
       <rgbColor rgb="ff1155cc"/>
     </indexedColors>
@@ -2073,35 +2271,39 @@
       <c r="D2" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" t="s" s="16">
+      <c r="E2" t="s" s="16">
         <v>19</v>
       </c>
+      <c r="F2" t="s" s="17">
+        <v>20</v>
+      </c>
       <c r="G2" t="s" s="16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s" s="16">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s" s="16">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s" s="16">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s" s="16">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s" s="17">
         <v>25</v>
       </c>
-      <c r="M2" t="s" s="18">
+      <c r="L2" t="s" s="18">
         <v>26</v>
       </c>
-      <c r="N2" t="s" s="18">
+      <c r="M2" t="s" s="19">
         <v>27</v>
       </c>
-      <c r="O2" s="19"/>
+      <c r="N2" t="s" s="19">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s" s="16">
+        <v>29</v>
+      </c>
       <c r="P2" s="20"/>
       <c r="Q2" s="21"/>
       <c r="R2" s="20"/>
@@ -2116,46 +2318,50 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="s" s="23">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s" s="24">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s" s="24">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="16">
         <v>18</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" t="s" s="16">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s" s="16">
-        <v>18</v>
+      <c r="E3" t="s" s="25">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s" s="27">
+        <v>35</v>
       </c>
       <c r="H3" t="s" s="16">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s" s="16">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s" s="16">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s" s="16">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s" s="17">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s" s="18">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s" s="18">
-        <v>34</v>
-      </c>
-      <c r="O3" s="19"/>
+        <v>39</v>
+      </c>
+      <c r="L3" t="s" s="18">
+        <v>26</v>
+      </c>
+      <c r="M3" t="s" s="19">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s" s="19">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s" s="16">
+        <v>42</v>
+      </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="21"/>
       <c r="R3" s="20"/>
@@ -2170,46 +2376,50 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="23">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s" s="24">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s" s="25">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s" s="26">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s" s="28">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s" s="17">
         <v>18</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" t="s" s="16">
-        <v>18</v>
+      <c r="E4" t="s" s="17">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s" s="29">
+        <v>47</v>
       </c>
       <c r="G4" t="s" s="16">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s" s="16">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s" s="16">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="J4" t="s" s="16">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="K4" t="s" s="16">
-        <v>39</v>
-      </c>
-      <c r="L4" t="s" s="17">
-        <v>25</v>
-      </c>
-      <c r="M4" t="s" s="18">
-        <v>40</v>
-      </c>
-      <c r="N4" t="s" s="18">
-        <v>41</v>
-      </c>
-      <c r="O4" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="L4" t="s" s="18">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s" s="19">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s" s="19">
+        <v>54</v>
+      </c>
+      <c r="O4" t="s" s="16">
+        <v>55</v>
+      </c>
       <c r="P4" s="20"/>
       <c r="Q4" s="21"/>
       <c r="R4" s="20"/>
@@ -2224,10 +2434,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="23">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s" s="24">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s" s="14">
         <v>17</v>
@@ -2235,8 +2445,10 @@
       <c r="D5" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" t="s" s="16">
+      <c r="E5" t="s" s="29">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="15">
         <v>18</v>
       </c>
       <c r="G5" t="s" s="16">
@@ -2248,12 +2460,16 @@
       <c r="I5" t="s" s="16">
         <v>18</v>
       </c>
-      <c r="J5" s="27"/>
+      <c r="J5" s="30"/>
       <c r="K5" s="16"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="19"/>
+      <c r="L5" s="18"/>
+      <c r="M5" t="s" s="19">
+        <v>58</v>
+      </c>
+      <c r="N5" s="31"/>
+      <c r="O5" t="s" s="16">
+        <v>59</v>
+      </c>
       <c r="P5" s="20"/>
       <c r="Q5" s="21"/>
       <c r="R5" s="20"/>
@@ -2268,72 +2484,80 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="23">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s" s="24">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s" s="24">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s" s="16">
         <v>18</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" t="s" s="16">
-        <v>47</v>
+      <c r="E6" t="s" s="15">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="17">
+        <v>63</v>
       </c>
       <c r="G6" t="s" s="16">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s" s="16">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s" s="16">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s" s="16">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s" s="16">
-        <v>52</v>
-      </c>
-      <c r="L6" t="s" s="17">
-        <v>53</v>
-      </c>
-      <c r="M6" s="18"/>
-      <c r="N6" t="s" s="18">
-        <v>54</v>
-      </c>
-      <c r="O6" s="19"/>
+        <v>68</v>
+      </c>
+      <c r="L6" t="s" s="18">
+        <v>69</v>
+      </c>
+      <c r="M6" t="s" s="19">
+        <v>70</v>
+      </c>
+      <c r="N6" t="s" s="19">
+        <v>71</v>
+      </c>
+      <c r="O6" t="s" s="16">
+        <v>72</v>
+      </c>
       <c r="P6" s="20"/>
       <c r="Q6" s="21"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="31"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="33"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="36"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="23">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s" s="16">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s" s="25">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s" s="28">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="26">
+      <c r="D7" t="s" s="17">
         <v>18</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" t="s" s="16">
-        <v>57</v>
+      <c r="E7" t="s" s="16">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s" s="15">
+        <v>76</v>
       </c>
       <c r="G7" t="s" s="16">
         <v>18</v>
@@ -2344,82 +2568,92 @@
       <c r="I7" t="s" s="16">
         <v>18</v>
       </c>
-      <c r="J7" s="27"/>
+      <c r="J7" s="30"/>
       <c r="K7" t="s" s="16">
-        <v>58</v>
-      </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="19"/>
+        <v>77</v>
+      </c>
+      <c r="L7" t="s" s="18">
+        <v>78</v>
+      </c>
+      <c r="M7" t="s" s="19">
+        <v>79</v>
+      </c>
+      <c r="N7" s="31"/>
+      <c r="O7" t="s" s="16">
+        <v>80</v>
+      </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="21"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="36"/>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="38"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="38"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="39"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="41"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="23">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s" s="24">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s" s="14">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" t="s" s="16">
+        <v>84</v>
+      </c>
       <c r="F8" t="s" s="16">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="G8" t="s" s="16">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s" s="16">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="I8" t="s" s="16">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="J8" t="s" s="16">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s" s="16">
-        <v>67</v>
-      </c>
-      <c r="L8" t="s" s="39">
-        <v>68</v>
-      </c>
-      <c r="M8" t="s" s="18">
-        <v>69</v>
-      </c>
-      <c r="N8" t="s" s="18">
-        <v>70</v>
-      </c>
-      <c r="O8" s="19"/>
+        <v>90</v>
+      </c>
+      <c r="L8" t="s" s="42">
+        <v>91</v>
+      </c>
+      <c r="M8" t="s" s="19">
+        <v>92</v>
+      </c>
+      <c r="N8" t="s" s="19">
+        <v>93</v>
+      </c>
+      <c r="O8" t="s" s="16">
+        <v>94</v>
+      </c>
       <c r="P8" s="20"/>
       <c r="Q8" s="21"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="36"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="33"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
+      <c r="V8" s="39"/>
+      <c r="W8" s="39"/>
+      <c r="X8" s="40"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="36"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="40"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="20"/>
       <c r="C9" s="24"/>
       <c r="D9" s="16"/>
@@ -2430,68 +2664,68 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="33"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="39"/>
+      <c r="U9" s="39"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="39"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="36"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="40"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="20"/>
       <c r="C10" s="24"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="27"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="47"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
       <c r="X10" s="9"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="33"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="36"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="40"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
@@ -2503,40 +2737,40 @@
       <c r="Z11" s="22"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="40"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="20"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="38"/>
-      <c r="Y12" s="47"/>
-      <c r="Z12" s="33"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="36"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="40"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="21"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -2559,95 +2793,95 @@
       <c r="Z13" s="22"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="40"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="42"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="21"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
-      <c r="L14" s="49"/>
+      <c r="L14" s="52"/>
       <c r="M14" s="20"/>
-      <c r="N14" s="50"/>
+      <c r="N14" s="53"/>
       <c r="O14" s="20"/>
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="30"/>
-      <c r="Z14" s="33"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="36"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="40"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="42"/>
+      <c r="E15" s="45"/>
       <c r="F15" s="21"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
-      <c r="L15" s="49"/>
+      <c r="L15" s="52"/>
       <c r="M15" s="20"/>
-      <c r="N15" s="19"/>
+      <c r="N15" s="54"/>
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
-      <c r="R15" s="34"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="33"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="38"/>
+      <c r="Z15" s="36"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="40"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="50"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="53"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="49"/>
+      <c r="L16" s="52"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="50"/>
+      <c r="N16" s="53"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
-      <c r="Q16" s="50"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="33"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="38"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="40"/>
+      <c r="Y16" s="38"/>
+      <c r="Z16" s="36"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="40"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
-      <c r="E17" s="42"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="21"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
@@ -2656,54 +2890,54 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
       <c r="M17" s="21"/>
-      <c r="N17" s="51"/>
+      <c r="N17" s="55"/>
       <c r="O17" s="20"/>
       <c r="P17" s="21"/>
       <c r="Q17" s="21"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="33"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="40"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="36"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="40"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="42"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="21"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="49"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="52"/>
       <c r="M18" s="20"/>
       <c r="N18" s="21"/>
       <c r="O18" s="20"/>
       <c r="P18" s="20"/>
       <c r="Q18" s="21"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="33"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="39"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="39"/>
+      <c r="W18" s="39"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="36"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="40"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="42"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="21"/>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
@@ -2716,22 +2950,22 @@
       <c r="O19" s="20"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="44"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="47"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
       <c r="W19" s="8"/>
       <c r="X19" s="9"/>
-      <c r="Y19" s="44"/>
-      <c r="Z19" s="33"/>
+      <c r="Y19" s="47"/>
+      <c r="Z19" s="36"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="40"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="42"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
@@ -2740,7 +2974,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
-      <c r="N20" s="50"/>
+      <c r="N20" s="53"/>
       <c r="O20" s="20"/>
       <c r="P20" s="20"/>
       <c r="Q20" s="20"/>
@@ -2755,11 +2989,11 @@
       <c r="Z20" s="22"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="40"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="42"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="21"/>
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
@@ -2783,11 +3017,11 @@
       <c r="Z21" s="22"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="40"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="42"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="21"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
@@ -2800,22 +3034,22 @@
       <c r="O22" s="20"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="30"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="33"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="33"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="33"/>
+      <c r="Z22" s="36"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="40"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="42"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="21"/>
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
@@ -2828,22 +3062,22 @@
       <c r="O23" s="20"/>
       <c r="P23" s="20"/>
       <c r="Q23" s="21"/>
-      <c r="R23" s="34"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="35"/>
-      <c r="Z23" s="33"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
+      <c r="V23" s="39"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="36"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="40"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="42"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="21"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
@@ -2856,50 +3090,50 @@
       <c r="O24" s="20"/>
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="33"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="39"/>
+      <c r="X24" s="40"/>
+      <c r="Y24" s="38"/>
+      <c r="Z24" s="36"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="40"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="42"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="21"/>
       <c r="G25" s="20"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20"/>
-      <c r="K25" s="53"/>
+      <c r="K25" s="57"/>
       <c r="L25" s="20"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="20"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="44"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="47"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
       <c r="X25" s="9"/>
-      <c r="Y25" s="44"/>
-      <c r="Z25" s="33"/>
+      <c r="Y25" s="47"/>
+      <c r="Z25" s="36"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="40"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
-      <c r="E26" s="42"/>
+      <c r="E26" s="45"/>
       <c r="F26" s="21"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
@@ -2923,19 +3157,19 @@
       <c r="Z26" s="22"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="40"/>
+      <c r="A27" s="43"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="42"/>
+      <c r="E27" s="45"/>
       <c r="F27" s="21"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
-      <c r="K27" s="19"/>
+      <c r="K27" s="54"/>
       <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
+      <c r="M27" s="45"/>
       <c r="N27" s="20"/>
       <c r="O27" s="20"/>
       <c r="P27" s="20"/>
@@ -2951,11 +3185,11 @@
       <c r="Z27" s="22"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="40"/>
+      <c r="A28" s="43"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
-      <c r="E28" s="42"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="21"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -2979,11 +3213,11 @@
       <c r="Z28" s="22"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="40"/>
+      <c r="A29" s="43"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="20"/>
-      <c r="E29" s="42"/>
+      <c r="E29" s="45"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -3007,11 +3241,11 @@
       <c r="Z29" s="22"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="40"/>
+      <c r="A30" s="43"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
-      <c r="E30" s="42"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="21"/>
       <c r="G30" s="20"/>
       <c r="H30" s="20"/>
@@ -3035,11 +3269,11 @@
       <c r="Z30" s="22"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="40"/>
+      <c r="A31" s="43"/>
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
-      <c r="E31" s="42"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="21"/>
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
@@ -3052,22 +3286,22 @@
       <c r="O31" s="20"/>
       <c r="P31" s="20"/>
       <c r="Q31" s="21"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="31"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="31"/>
-      <c r="X31" s="32"/>
-      <c r="Y31" s="30"/>
-      <c r="Z31" s="33"/>
+      <c r="R31" s="32"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="34"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
+      <c r="X31" s="35"/>
+      <c r="Y31" s="33"/>
+      <c r="Z31" s="36"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="40"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
-      <c r="E32" s="42"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -3080,28 +3314,28 @@
       <c r="O32" s="20"/>
       <c r="P32" s="21"/>
       <c r="Q32" s="21"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="44"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="47"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
       <c r="V32" s="8"/>
       <c r="W32" s="8"/>
       <c r="X32" s="9"/>
-      <c r="Y32" s="44"/>
-      <c r="Z32" s="33"/>
+      <c r="Y32" s="47"/>
+      <c r="Z32" s="36"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="40"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="D33" s="20"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="54"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="58"/>
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="49"/>
+      <c r="K33" s="52"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
       <c r="N33" s="20"/>
@@ -3119,11 +3353,11 @@
       <c r="Z33" s="22"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="40"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
-      <c r="E34" s="42"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="21"/>
       <c r="G34" s="20"/>
       <c r="H34" s="20"/>
@@ -3147,11 +3381,11 @@
       <c r="Z34" s="22"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="40"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
       <c r="D35" s="20"/>
-      <c r="E35" s="42"/>
+      <c r="E35" s="45"/>
       <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="H35" s="20"/>
@@ -3175,11 +3409,11 @@
       <c r="Z35" s="22"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="40"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
-      <c r="E36" s="42"/>
+      <c r="E36" s="45"/>
       <c r="F36" s="21"/>
       <c r="G36" s="20"/>
       <c r="H36" s="20"/>
@@ -3203,7 +3437,7 @@
       <c r="Z36" s="22"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="55"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
@@ -3220,18 +3454,18 @@
       <c r="O37" s="20"/>
       <c r="P37" s="20"/>
       <c r="Q37" s="20"/>
-      <c r="R37" s="29"/>
-      <c r="S37" s="56"/>
-      <c r="T37" s="56"/>
-      <c r="U37" s="56"/>
-      <c r="V37" s="56"/>
-      <c r="W37" s="56"/>
-      <c r="X37" s="56"/>
-      <c r="Y37" s="57"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="60"/>
+      <c r="W37" s="60"/>
+      <c r="X37" s="60"/>
+      <c r="Y37" s="61"/>
       <c r="Z37" s="22"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="40"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -3248,18 +3482,18 @@
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
       <c r="Q38" s="21"/>
-      <c r="R38" s="43"/>
-      <c r="S38" s="44"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="47"/>
       <c r="T38" s="8"/>
       <c r="U38" s="8"/>
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
       <c r="X38" s="9"/>
-      <c r="Y38" s="44"/>
-      <c r="Z38" s="33"/>
+      <c r="Y38" s="47"/>
+      <c r="Z38" s="36"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="40"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20"/>
       <c r="D39" s="20"/>
@@ -3287,7 +3521,7 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="40"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -3304,18 +3538,18 @@
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
       <c r="Q40" s="21"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="30"/>
-      <c r="T40" s="31"/>
-      <c r="U40" s="31"/>
-      <c r="V40" s="31"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="32"/>
-      <c r="Y40" s="30"/>
-      <c r="Z40" s="33"/>
+      <c r="R40" s="32"/>
+      <c r="S40" s="33"/>
+      <c r="T40" s="34"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="34"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="33"/>
+      <c r="Z40" s="36"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="40"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
@@ -3326,24 +3560,24 @@
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
-      <c r="L41" s="49"/>
+      <c r="L41" s="52"/>
       <c r="M41" s="20"/>
       <c r="N41" s="20"/>
       <c r="O41" s="20"/>
       <c r="P41" s="21"/>
       <c r="Q41" s="21"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="44"/>
+      <c r="R41" s="46"/>
+      <c r="S41" s="47"/>
       <c r="T41" s="8"/>
       <c r="U41" s="8"/>
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
       <c r="X41" s="9"/>
-      <c r="Y41" s="44"/>
-      <c r="Z41" s="33"/>
+      <c r="Y41" s="47"/>
+      <c r="Z41" s="36"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="40"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
       <c r="D42" s="20"/>
@@ -3353,7 +3587,7 @@
       <c r="H42" s="20"/>
       <c r="I42" s="20"/>
       <c r="J42" s="20"/>
-      <c r="K42" s="49"/>
+      <c r="K42" s="52"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
       <c r="N42" s="20"/>
@@ -3371,7 +3605,7 @@
       <c r="Z42" s="22"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="40"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
@@ -3388,18 +3622,18 @@
       <c r="O43" s="20"/>
       <c r="P43" s="20"/>
       <c r="Q43" s="21"/>
-      <c r="R43" s="46"/>
-      <c r="S43" s="47"/>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-      <c r="V43" s="48"/>
-      <c r="W43" s="48"/>
-      <c r="X43" s="38"/>
-      <c r="Y43" s="47"/>
-      <c r="Z43" s="33"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="50"/>
+      <c r="T43" s="51"/>
+      <c r="U43" s="51"/>
+      <c r="V43" s="51"/>
+      <c r="W43" s="51"/>
+      <c r="X43" s="41"/>
+      <c r="Y43" s="50"/>
+      <c r="Z43" s="36"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="58"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
@@ -3410,9 +3644,9 @@
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
-      <c r="L44" s="49"/>
+      <c r="L44" s="52"/>
       <c r="M44" s="20"/>
-      <c r="N44" s="50"/>
+      <c r="N44" s="53"/>
       <c r="O44" s="20"/>
       <c r="P44" s="20"/>
       <c r="Q44" s="21"/>
@@ -3427,7 +3661,7 @@
       <c r="Z44" s="22"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="40"/>
+      <c r="A45" s="43"/>
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
@@ -3437,25 +3671,25 @@
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
-      <c r="K45" s="49"/>
+      <c r="K45" s="52"/>
       <c r="L45" s="20"/>
       <c r="M45" s="21"/>
       <c r="N45" s="21"/>
       <c r="O45" s="20"/>
       <c r="P45" s="21"/>
       <c r="Q45" s="21"/>
-      <c r="R45" s="29"/>
-      <c r="S45" s="30"/>
-      <c r="T45" s="31"/>
-      <c r="U45" s="31"/>
-      <c r="V45" s="31"/>
-      <c r="W45" s="31"/>
-      <c r="X45" s="32"/>
-      <c r="Y45" s="30"/>
-      <c r="Z45" s="33"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="33"/>
+      <c r="T45" s="34"/>
+      <c r="U45" s="34"/>
+      <c r="V45" s="34"/>
+      <c r="W45" s="34"/>
+      <c r="X45" s="35"/>
+      <c r="Y45" s="33"/>
+      <c r="Z45" s="36"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="40"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -3472,18 +3706,18 @@
       <c r="O46" s="20"/>
       <c r="P46" s="20"/>
       <c r="Q46" s="21"/>
-      <c r="R46" s="34"/>
-      <c r="S46" s="35"/>
-      <c r="T46" s="36"/>
-      <c r="U46" s="36"/>
-      <c r="V46" s="36"/>
-      <c r="W46" s="36"/>
-      <c r="X46" s="37"/>
-      <c r="Y46" s="35"/>
-      <c r="Z46" s="33"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="38"/>
+      <c r="T46" s="39"/>
+      <c r="U46" s="39"/>
+      <c r="V46" s="39"/>
+      <c r="W46" s="39"/>
+      <c r="X46" s="40"/>
+      <c r="Y46" s="38"/>
+      <c r="Z46" s="36"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="40"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
@@ -3500,18 +3734,18 @@
       <c r="O47" s="20"/>
       <c r="P47" s="21"/>
       <c r="Q47" s="21"/>
-      <c r="R47" s="34"/>
-      <c r="S47" s="35"/>
-      <c r="T47" s="36"/>
-      <c r="U47" s="36"/>
-      <c r="V47" s="36"/>
-      <c r="W47" s="36"/>
-      <c r="X47" s="37"/>
-      <c r="Y47" s="35"/>
-      <c r="Z47" s="33"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="38"/>
+      <c r="T47" s="39"/>
+      <c r="U47" s="39"/>
+      <c r="V47" s="39"/>
+      <c r="W47" s="39"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="38"/>
+      <c r="Z47" s="36"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="40"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
@@ -3528,18 +3762,18 @@
       <c r="O48" s="20"/>
       <c r="P48" s="21"/>
       <c r="Q48" s="21"/>
-      <c r="R48" s="34"/>
-      <c r="S48" s="35"/>
-      <c r="T48" s="36"/>
-      <c r="U48" s="36"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="37"/>
-      <c r="Y48" s="35"/>
-      <c r="Z48" s="33"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="38"/>
+      <c r="T48" s="39"/>
+      <c r="U48" s="39"/>
+      <c r="V48" s="39"/>
+      <c r="W48" s="39"/>
+      <c r="X48" s="40"/>
+      <c r="Y48" s="38"/>
+      <c r="Z48" s="36"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="40"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
@@ -3552,22 +3786,22 @@
       <c r="K49" s="20"/>
       <c r="L49" s="20"/>
       <c r="M49" s="20"/>
-      <c r="N49" s="50"/>
+      <c r="N49" s="53"/>
       <c r="O49" s="20"/>
       <c r="P49" s="21"/>
       <c r="Q49" s="21"/>
-      <c r="R49" s="34"/>
-      <c r="S49" s="35"/>
-      <c r="T49" s="36"/>
-      <c r="U49" s="36"/>
-      <c r="V49" s="36"/>
-      <c r="W49" s="36"/>
-      <c r="X49" s="37"/>
-      <c r="Y49" s="35"/>
-      <c r="Z49" s="33"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="38"/>
+      <c r="T49" s="39"/>
+      <c r="U49" s="39"/>
+      <c r="V49" s="39"/>
+      <c r="W49" s="39"/>
+      <c r="X49" s="40"/>
+      <c r="Y49" s="38"/>
+      <c r="Z49" s="36"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="40"/>
+      <c r="A50" s="43"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
@@ -3584,20 +3818,20 @@
       <c r="O50" s="20"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="20"/>
-      <c r="R50" s="34"/>
-      <c r="S50" s="35"/>
-      <c r="T50" s="36"/>
-      <c r="U50" s="36"/>
-      <c r="V50" s="36"/>
-      <c r="W50" s="36"/>
-      <c r="X50" s="37"/>
-      <c r="Y50" s="35"/>
-      <c r="Z50" s="33"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="38"/>
+      <c r="T50" s="39"/>
+      <c r="U50" s="39"/>
+      <c r="V50" s="39"/>
+      <c r="W50" s="39"/>
+      <c r="X50" s="40"/>
+      <c r="Y50" s="38"/>
+      <c r="Z50" s="36"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="40"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="20"/>
-      <c r="C51" s="19"/>
+      <c r="C51" s="54"/>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
       <c r="F51" s="21"/>
@@ -3608,22 +3842,22 @@
       <c r="K51" s="20"/>
       <c r="L51" s="20"/>
       <c r="M51" s="21"/>
-      <c r="N51" s="50"/>
+      <c r="N51" s="53"/>
       <c r="O51" s="20"/>
       <c r="P51" s="21"/>
       <c r="Q51" s="21"/>
-      <c r="R51" s="43"/>
-      <c r="S51" s="44"/>
+      <c r="R51" s="46"/>
+      <c r="S51" s="47"/>
       <c r="T51" s="8"/>
       <c r="U51" s="8"/>
       <c r="V51" s="8"/>
       <c r="W51" s="8"/>
       <c r="X51" s="9"/>
-      <c r="Y51" s="44"/>
-      <c r="Z51" s="33"/>
+      <c r="Y51" s="47"/>
+      <c r="Z51" s="36"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="40"/>
+      <c r="A52" s="43"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
@@ -3651,7 +3885,7 @@
       <c r="Z52" s="22"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="40"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
@@ -3679,7 +3913,7 @@
       <c r="Z53" s="22"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="40"/>
+      <c r="A54" s="43"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
@@ -3696,18 +3930,18 @@
       <c r="O54" s="20"/>
       <c r="P54" s="20"/>
       <c r="Q54" s="21"/>
-      <c r="R54" s="29"/>
-      <c r="S54" s="30"/>
-      <c r="T54" s="31"/>
-      <c r="U54" s="31"/>
-      <c r="V54" s="31"/>
-      <c r="W54" s="31"/>
-      <c r="X54" s="32"/>
-      <c r="Y54" s="30"/>
-      <c r="Z54" s="33"/>
+      <c r="R54" s="32"/>
+      <c r="S54" s="33"/>
+      <c r="T54" s="34"/>
+      <c r="U54" s="34"/>
+      <c r="V54" s="34"/>
+      <c r="W54" s="34"/>
+      <c r="X54" s="35"/>
+      <c r="Y54" s="33"/>
+      <c r="Z54" s="36"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="40"/>
+      <c r="A55" s="43"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
       <c r="D55" s="20"/>
@@ -3724,18 +3958,18 @@
       <c r="O55" s="20"/>
       <c r="P55" s="21"/>
       <c r="Q55" s="21"/>
-      <c r="R55" s="34"/>
-      <c r="S55" s="35"/>
-      <c r="T55" s="36"/>
-      <c r="U55" s="36"/>
-      <c r="V55" s="36"/>
-      <c r="W55" s="36"/>
-      <c r="X55" s="37"/>
-      <c r="Y55" s="35"/>
-      <c r="Z55" s="33"/>
+      <c r="R55" s="37"/>
+      <c r="S55" s="38"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="39"/>
+      <c r="V55" s="39"/>
+      <c r="W55" s="39"/>
+      <c r="X55" s="40"/>
+      <c r="Y55" s="38"/>
+      <c r="Z55" s="36"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="40"/>
+      <c r="A56" s="43"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -3752,18 +3986,18 @@
       <c r="O56" s="20"/>
       <c r="P56" s="21"/>
       <c r="Q56" s="21"/>
-      <c r="R56" s="34"/>
-      <c r="S56" s="35"/>
-      <c r="T56" s="36"/>
-      <c r="U56" s="36"/>
-      <c r="V56" s="36"/>
-      <c r="W56" s="36"/>
-      <c r="X56" s="37"/>
-      <c r="Y56" s="35"/>
-      <c r="Z56" s="33"/>
+      <c r="R56" s="37"/>
+      <c r="S56" s="38"/>
+      <c r="T56" s="39"/>
+      <c r="U56" s="39"/>
+      <c r="V56" s="39"/>
+      <c r="W56" s="39"/>
+      <c r="X56" s="40"/>
+      <c r="Y56" s="38"/>
+      <c r="Z56" s="36"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="40"/>
+      <c r="A57" s="43"/>
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
       <c r="D57" s="20"/>
@@ -3776,22 +4010,22 @@
       <c r="K57" s="20"/>
       <c r="L57" s="20"/>
       <c r="M57" s="21"/>
-      <c r="N57" s="59"/>
+      <c r="N57" s="63"/>
       <c r="O57" s="20"/>
       <c r="P57" s="21"/>
       <c r="Q57" s="21"/>
-      <c r="R57" s="43"/>
-      <c r="S57" s="44"/>
+      <c r="R57" s="46"/>
+      <c r="S57" s="47"/>
       <c r="T57" s="8"/>
       <c r="U57" s="8"/>
       <c r="V57" s="8"/>
       <c r="W57" s="8"/>
       <c r="X57" s="9"/>
-      <c r="Y57" s="44"/>
-      <c r="Z57" s="33"/>
+      <c r="Y57" s="47"/>
+      <c r="Z57" s="36"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="40"/>
+      <c r="A58" s="43"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
@@ -3819,7 +4053,7 @@
       <c r="Z58" s="22"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="40"/>
+      <c r="A59" s="43"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
       <c r="D59" s="20"/>
@@ -3847,7 +4081,7 @@
       <c r="Z59" s="22"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="40"/>
+      <c r="A60" s="43"/>
       <c r="B60" s="20"/>
       <c r="C60" s="20"/>
       <c r="D60" s="20"/>
@@ -3875,7 +4109,7 @@
       <c r="Z60" s="22"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="40"/>
+      <c r="A61" s="43"/>
       <c r="B61" s="20"/>
       <c r="C61" s="20"/>
       <c r="D61" s="20"/>
@@ -3903,7 +4137,7 @@
       <c r="Z61" s="22"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="40"/>
+      <c r="A62" s="43"/>
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
       <c r="D62" s="20"/>
@@ -3931,7 +4165,7 @@
       <c r="Z62" s="22"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="40"/>
+      <c r="A63" s="43"/>
       <c r="B63" s="20"/>
       <c r="C63" s="20"/>
       <c r="D63" s="20"/>
@@ -3959,7 +4193,7 @@
       <c r="Z63" s="22"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="40"/>
+      <c r="A64" s="43"/>
       <c r="B64" s="20"/>
       <c r="C64" s="20"/>
       <c r="D64" s="20"/>
@@ -3987,7 +4221,7 @@
       <c r="Z64" s="22"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="40"/>
+      <c r="A65" s="43"/>
       <c r="B65" s="20"/>
       <c r="C65" s="20"/>
       <c r="D65" s="20"/>
@@ -4015,7 +4249,7 @@
       <c r="Z65" s="22"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="40"/>
+      <c r="A66" s="43"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20"/>
       <c r="D66" s="20"/>
@@ -4043,7 +4277,7 @@
       <c r="Z66" s="22"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="40"/>
+      <c r="A67" s="43"/>
       <c r="B67" s="20"/>
       <c r="C67" s="20"/>
       <c r="D67" s="20"/>
@@ -4071,34 +4305,40 @@
       <c r="Z67" s="22"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="60"/>
-      <c r="B68" s="61"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="61"/>
-      <c r="G68" s="61"/>
-      <c r="H68" s="61"/>
-      <c r="I68" s="61"/>
-      <c r="J68" s="61"/>
-      <c r="K68" s="61"/>
-      <c r="L68" s="61"/>
-      <c r="M68" s="61"/>
-      <c r="N68" s="61"/>
-      <c r="O68" s="61"/>
-      <c r="P68" s="61"/>
-      <c r="Q68" s="61"/>
-      <c r="R68" s="61"/>
-      <c r="S68" s="61"/>
-      <c r="T68" s="61"/>
-      <c r="U68" s="61"/>
-      <c r="V68" s="61"/>
-      <c r="W68" s="61"/>
-      <c r="X68" s="61"/>
-      <c r="Y68" s="61"/>
-      <c r="Z68" s="62"/>
+      <c r="A68" s="64"/>
+      <c r="B68" s="65"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="65"/>
+      <c r="F68" s="65"/>
+      <c r="G68" s="65"/>
+      <c r="H68" s="65"/>
+      <c r="I68" s="65"/>
+      <c r="J68" s="65"/>
+      <c r="K68" s="65"/>
+      <c r="L68" s="65"/>
+      <c r="M68" s="65"/>
+      <c r="N68" s="65"/>
+      <c r="O68" s="65"/>
+      <c r="P68" s="65"/>
+      <c r="Q68" s="65"/>
+      <c r="R68" s="65"/>
+      <c r="S68" s="65"/>
+      <c r="T68" s="65"/>
+      <c r="U68" s="65"/>
+      <c r="V68" s="65"/>
+      <c r="W68" s="65"/>
+      <c r="X68" s="65"/>
+      <c r="Y68" s="65"/>
+      <c r="Z68" s="66"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="E3" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="E4" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="E8" r:id="rId4" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>